<commit_message>
Add: tai lieu + Update: admin folder
</commit_message>
<xml_diff>
--- a/tai_lieu/Sơ đồ cơ sở dữ liệu - BÁN HÀNG.xlsx
+++ b/tai_lieu/Sơ đồ cơ sở dữ liệu - BÁN HÀNG.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\j2school_Project\tai_lieu\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF9182B-E851-4528-AC9E-6117152CF249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Trang tính1" sheetId="1" r:id="rId4"/>
+    <sheet name="Trang tính1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
   <si>
     <t>DỮ LIỆU WEBSITE CỬA HÀNG BÁNH</t>
   </si>
@@ -110,32 +119,50 @@
   </si>
   <si>
     <t>ghi_chu</t>
+  </si>
+  <si>
+    <t>discount</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="14.0"/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -143,11 +170,17 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
-    <border/>
+  <borders count="3">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -161,42 +194,59 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="10">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -386,190 +436,210 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A2:J22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="17.71"/>
-    <col customWidth="1" min="3" max="3" width="19.14"/>
-    <col customWidth="1" min="5" max="5" width="19.0"/>
-    <col customWidth="1" min="7" max="7" width="19.14"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="s">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="2" t="s">
+      <c r="B4" s="2"/>
+      <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="2" t="s">
+      <c r="D4" s="2"/>
+      <c r="E4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="2" t="s">
+      <c r="F4" s="2"/>
+      <c r="G4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="4" t="s">
+      <c r="B10" s="4"/>
+      <c r="C10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11">
-      <c r="C11" s="4" t="s">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12">
-      <c r="D12" s="5" t="s">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D12" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="2" t="s">
+    <row r="14" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="2" t="s">
+      <c r="B14" s="2"/>
+      <c r="C14" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="4" t="s">
+      <c r="E14" s="7"/>
+      <c r="J14" s="8"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="4" t="s">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="4" t="s">
+      <c r="E16" s="8"/>
+    </row>
+    <row r="17" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="4" t="s">
+    <row r="18" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="4" t="s">
+    <row r="19" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="4" t="s">
+    <row r="20" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="4" t="s">
+    <row r="21" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="9" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A2:G2"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update: css + excel
</commit_message>
<xml_diff>
--- a/tai_lieu/Sơ đồ cơ sở dữ liệu - BÁN HÀNG.xlsx
+++ b/tai_lieu/Sơ đồ cơ sở dữ liệu - BÁN HÀNG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\j2school_Project\tai_lieu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF9182B-E851-4528-AC9E-6117152CF249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{480AB85F-3DAF-475B-8099-F16E7B8E78DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -221,13 +221,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,10 +446,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A2:J22"/>
+  <dimension ref="A2:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -461,17 +461,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+    </row>
+    <row r="4" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -488,7 +488,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -502,7 +502,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -516,7 +516,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
@@ -527,7 +527,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
@@ -538,7 +538,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
@@ -549,7 +549,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>17</v>
       </c>
@@ -561,7 +561,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C11" s="3" t="s">
         <v>19</v>
       </c>
@@ -569,7 +569,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="D12" s="4" t="s">
         <v>21</v>
       </c>
@@ -582,10 +582,10 @@
       <c r="C14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E14" s="7"/>
-      <c r="J14" s="8"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E14" s="5"/>
+      <c r="J14" s="6"/>
+    </row>
+    <row r="15" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>5</v>
       </c>
@@ -593,14 +593,14 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="8"/>
+      <c r="E16" s="6"/>
     </row>
     <row r="17" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
@@ -614,6 +614,9 @@
       <c r="A18" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="C18" s="7" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="19" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
@@ -628,11 +631,6 @@
     <row r="21" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="9" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: sua lai file bang du lieu
</commit_message>
<xml_diff>
--- a/tai_lieu/Sơ đồ cơ sở dữ liệu - BÁN HÀNG.xlsx
+++ b/tai_lieu/Sơ đồ cơ sở dữ liệu - BÁN HÀNG.xlsx
@@ -8,19 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\j2school_Project\tai_lieu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{480AB85F-3DAF-475B-8099-F16E7B8E78DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{663D85C7-9F99-468B-9970-359618AAC668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="513" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Trang tính1" sheetId="1" r:id="rId1"/>
+    <sheet name="bảng dữ liệu" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
   <si>
     <t>DỮ LIỆU WEBSITE CỬA HÀNG BÁNH</t>
   </si>
@@ -121,7 +130,16 @@
     <t>ghi_chu</t>
   </si>
   <si>
-    <t>discount</t>
+    <t>giam_gia</t>
+  </si>
+  <si>
+    <t>1,2,3…</t>
+  </si>
+  <si>
+    <t>phan_tram</t>
+  </si>
+  <si>
+    <t>ma_cap_do</t>
   </si>
 </sst>
 </file>
@@ -173,7 +191,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -211,19 +229,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -449,7 +483,7 @@
   <dimension ref="A2:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D9" activeCellId="2" sqref="E15 E12 D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -461,15 +495,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
     </row>
     <row r="4" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -550,7 +584,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="7" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="4"/>
@@ -562,6 +596,12 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
       <c r="C11" s="3" t="s">
         <v>19</v>
       </c>
@@ -582,8 +622,10 @@
       <c r="C14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E14" s="5"/>
-      <c r="J14" s="6"/>
+      <c r="E14" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
@@ -592,6 +634,9 @@
       <c r="C15" s="3" t="s">
         <v>24</v>
       </c>
+      <c r="E15" s="6" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="16" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
@@ -600,7 +645,9 @@
       <c r="C16" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="6"/>
+      <c r="E16" s="10" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="17" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
@@ -613,9 +660,6 @@
     <row r="18" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fix: chinh sua CRUD
</commit_message>
<xml_diff>
--- a/tai_lieu/Sơ đồ cơ sở dữ liệu - BÁN HÀNG.xlsx
+++ b/tai_lieu/Sơ đồ cơ sở dữ liệu - BÁN HÀNG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\j2school_Project\tai_lieu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{663D85C7-9F99-468B-9970-359618AAC668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A259223-B011-4D0D-9CC5-82B4F329D732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="513" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,9 +46,6 @@
     <t>san_pham</t>
   </si>
   <si>
-    <t>ma</t>
-  </si>
-  <si>
     <t>ten</t>
   </si>
   <si>
@@ -139,7 +136,10 @@
     <t>phan_tram</t>
   </si>
   <si>
-    <t>ma_cap_do</t>
+    <t>ma🔑</t>
+  </si>
+  <si>
+    <t>ma_cap_do🔑</t>
   </si>
 </sst>
 </file>
@@ -483,7 +483,7 @@
   <dimension ref="A2:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" activeCellId="2" sqref="E15 E12 D9"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -524,126 +524,126 @@
     </row>
     <row r="5" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="G6" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="G7" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="G8" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="B11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="D12" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="E16" s="10" t="s">
         <v>36</v>
@@ -651,30 +651,30 @@
     </row>
     <row r="17" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update: chinh sua tai lieu
</commit_message>
<xml_diff>
--- a/tai_lieu/Sơ đồ cơ sở dữ liệu - BÁN HÀNG.xlsx
+++ b/tai_lieu/Sơ đồ cơ sở dữ liệu - BÁN HÀNG.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\j2school_Project\tai_lieu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A259223-B011-4D0D-9CC5-82B4F329D732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC4DDC90-9F2C-460C-BD73-7693D5F0E5AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="513" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
   <si>
     <t>DỮ LIỆU WEBSITE CỬA HÀNG BÁNH</t>
   </si>
@@ -130,9 +130,6 @@
     <t>giam_gia</t>
   </si>
   <si>
-    <t>1,2,3…</t>
-  </si>
-  <si>
     <t>phan_tram</t>
   </si>
   <si>
@@ -140,6 +137,15 @@
   </si>
   <si>
     <t>ma_cap_do🔑</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>tong_tien</t>
+  </si>
+  <si>
+    <t>trang_thai</t>
   </si>
 </sst>
 </file>
@@ -191,7 +197,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -242,11 +248,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -261,7 +278,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -480,15 +498,16 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A2:J21"/>
+  <dimension ref="A2:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
     <col min="3" max="3" width="19.140625" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
     <col min="7" max="7" width="19.140625" customWidth="1"/>
@@ -498,188 +517,214 @@
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-    </row>
-    <row r="4" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+    </row>
+    <row r="4" spans="1:10" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="1" t="s">
+      <c r="C5" s="2"/>
+      <c r="D5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="1" t="s">
+      <c r="E5" s="2"/>
+      <c r="F5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="1" t="s">
+      <c r="G5" s="2"/>
+      <c r="H5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+    <row r="6" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B11" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B12" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B14" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J14" s="5"/>
+    </row>
+    <row r="15" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:10" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="17" spans="2:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" t="s">
+    </row>
+    <row r="19" spans="2:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D12" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="J14" s="5"/>
-    </row>
-    <row r="15" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E16" s="10" t="s">
+    </row>
+    <row r="20" spans="2:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B20" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="3" t="s">
+      <c r="D20" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
+      <c r="F20" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B21" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
+    <row r="22" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
+    <row r="23" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
+    <row r="24" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="7" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="8" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>